<commit_message>
Update New Reader & Refactor unused imports.
</commit_message>
<xml_diff>
--- a/data/src/site/KOD AKAUN HASIL YURAN PELAJAR PASCASISWAZAH 2015.xlsx
+++ b/data/src/site/KOD AKAUN HASIL YURAN PELAJAR PASCASISWAZAH 2015.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20730" windowHeight="9525"/>
+    <workbookView xWindow="285" yWindow="135" windowWidth="9690" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>YURAN PENDAFTARAN</t>
   </si>
@@ -85,9 +85,6 @@
     <t>TABPPS-PCA-00-H79329</t>
   </si>
   <si>
-    <t>YURAN PENYELIDIKAN</t>
-  </si>
-  <si>
     <t>TABPPS-PCA-00-H79332</t>
   </si>
   <si>
@@ -155,6 +152,15 @@
   </si>
   <si>
     <t>PPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YURAN PENYELIDIKAN/Yuran Pengajian </t>
+  </si>
+  <si>
+    <t>TABPPS-PCA-00-H79336</t>
+  </si>
+  <si>
+    <t>BENCH FEES</t>
   </si>
 </sst>
 </file>
@@ -1594,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1613,7 +1619,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="G1" s="1"/>
@@ -1622,7 +1628,7 @@
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1638,7 +1644,7 @@
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
@@ -1670,7 +1676,7 @@
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -1683,7 +1689,7 @@
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -1699,7 +1705,7 @@
     </row>
     <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -1715,7 +1721,7 @@
     </row>
     <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -1743,7 +1749,7 @@
     </row>
     <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
@@ -1759,7 +1765,7 @@
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
@@ -1775,7 +1781,7 @@
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>2</v>
@@ -1791,7 +1797,7 @@
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>3</v>
@@ -1804,7 +1810,7 @@
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
@@ -1820,7 +1826,7 @@
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
@@ -1836,7 +1842,7 @@
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>6</v>
@@ -1888,7 +1894,7 @@
     </row>
     <row r="20" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="5"/>
@@ -2033,7 +2039,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4"/>
@@ -2043,7 +2049,7 @@
     </row>
     <row r="31" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>6</v>
@@ -2056,10 +2062,10 @@
     </row>
     <row r="32" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="4"/>
@@ -2069,10 +2075,10 @@
     </row>
     <row r="33" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
@@ -2080,10 +2086,10 @@
     </row>
     <row r="34" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="4"/>
@@ -2091,6 +2097,12 @@
       <c r="M34" s="5"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="M35" s="3"/>
     </row>

</xml_diff>